<commit_message>
Updated Bug Metric Document
</commit_message>
<xml_diff>
--- a/Bug Log & Metric.xlsx
+++ b/Bug Log & Metric.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FYP\venv\Beyond-Ideas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A36FF3D-9CEE-4138-8A5C-299DDBCA5A9D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E490ABC-BD77-457C-A9E7-45EF28D646EA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="438" windowWidth="28800" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -570,15 +570,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -592,6 +583,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1590,7 +1590,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-SG" sz="1400" b="1"/>
-            <a:t>Iterations</a:t>
+            <a:t>Iteration</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1899,8 +1899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1916,13 +1916,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="60"/>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="59"/>
+      <c r="A1" s="63"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="65"/>
       <c r="H1" s="1"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -1944,25 +1944,25 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="62" t="s">
+      <c r="C2" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="62" t="s">
+      <c r="D2" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="62" t="s">
+      <c r="E2" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="62" t="s">
+      <c r="F2" s="59" t="s">
         <v>39</v>
       </c>
-      <c r="G2" s="62" t="s">
+      <c r="G2" s="59" t="s">
         <v>21</v>
       </c>
       <c r="H2" s="3"/>
@@ -1990,25 +1990,25 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A3" s="61">
+      <c r="A3" s="58">
         <v>1</v>
       </c>
-      <c r="B3" s="63">
+      <c r="B3" s="60">
         <v>0</v>
       </c>
-      <c r="C3" s="63">
+      <c r="C3" s="60">
         <v>0</v>
       </c>
-      <c r="D3" s="63">
+      <c r="D3" s="60">
         <v>0</v>
       </c>
-      <c r="E3" s="63">
+      <c r="E3" s="60">
         <v>0</v>
       </c>
-      <c r="F3" s="63">
+      <c r="F3" s="60">
         <v>0</v>
       </c>
-      <c r="G3" s="64" t="s">
+      <c r="G3" s="61" t="s">
         <v>38</v>
       </c>
       <c r="H3" s="3"/>
@@ -2036,25 +2036,25 @@
       <c r="Z3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A4" s="61">
+      <c r="A4" s="58">
         <v>2</v>
       </c>
-      <c r="B4" s="65">
+      <c r="B4" s="62">
         <v>0</v>
       </c>
-      <c r="C4" s="63">
+      <c r="C4" s="60">
         <v>0</v>
       </c>
-      <c r="D4" s="65">
+      <c r="D4" s="62">
         <v>0</v>
       </c>
-      <c r="E4" s="65">
+      <c r="E4" s="62">
         <v>0</v>
       </c>
-      <c r="F4" s="65">
+      <c r="F4" s="62">
         <v>0</v>
       </c>
-      <c r="G4" s="64" t="s">
+      <c r="G4" s="61" t="s">
         <v>38</v>
       </c>
       <c r="H4" s="3"/>
@@ -2082,15 +2082,15 @@
       <c r="Z4" s="1"/>
     </row>
     <row r="5" spans="1:26" ht="13.8" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A5" s="61">
+      <c r="A5" s="58">
         <v>3</v>
       </c>
-      <c r="B5" s="63"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63"/>
-      <c r="G5" s="64"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="61"/>
       <c r="H5" s="3"/>
       <c r="I5" s="4" t="s">
         <v>27</v>
@@ -2116,15 +2116,15 @@
       <c r="Z5" s="1"/>
     </row>
     <row r="6" spans="1:26" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A6" s="61">
+      <c r="A6" s="58">
         <v>4</v>
       </c>
-      <c r="B6" s="63"/>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
-      <c r="G6" s="64"/>
+      <c r="B6" s="60"/>
+      <c r="C6" s="60"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="60"/>
+      <c r="F6" s="60"/>
+      <c r="G6" s="61"/>
       <c r="H6" s="6"/>
       <c r="I6" s="14"/>
       <c r="J6" s="15"/>
@@ -2146,15 +2146,15 @@
       <c r="Z6" s="1"/>
     </row>
     <row r="7" spans="1:26" ht="14.4" x14ac:dyDescent="0.4">
-      <c r="A7" s="61">
+      <c r="A7" s="58">
         <v>5</v>
       </c>
-      <c r="B7" s="63"/>
-      <c r="C7" s="63"/>
-      <c r="D7" s="63"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="63"/>
-      <c r="G7" s="64"/>
+      <c r="B7" s="60"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
+      <c r="G7" s="61"/>
       <c r="H7" s="1"/>
       <c r="I7" s="55" t="s">
         <v>29</v>
@@ -2178,15 +2178,15 @@
       <c r="Z7" s="1"/>
     </row>
     <row r="8" spans="1:26" ht="14.4" x14ac:dyDescent="0.4">
-      <c r="A8" s="61">
+      <c r="A8" s="58">
         <v>6</v>
       </c>
-      <c r="B8" s="63"/>
-      <c r="C8" s="63"/>
-      <c r="D8" s="63"/>
-      <c r="E8" s="63"/>
-      <c r="F8" s="63"/>
-      <c r="G8" s="64"/>
+      <c r="B8" s="60"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="60"/>
+      <c r="G8" s="61"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -2208,15 +2208,15 @@
       <c r="Z8" s="1"/>
     </row>
     <row r="9" spans="1:26" ht="14.4" x14ac:dyDescent="0.4">
-      <c r="A9" s="61">
+      <c r="A9" s="58">
         <v>7</v>
       </c>
-      <c r="B9" s="63"/>
-      <c r="C9" s="63"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="63"/>
-      <c r="G9" s="64"/>
+      <c r="B9" s="60"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="61"/>
       <c r="H9" s="1"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -2238,15 +2238,15 @@
       <c r="Z9" s="1"/>
     </row>
     <row r="10" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A10" s="61">
+      <c r="A10" s="58">
         <v>8</v>
       </c>
-      <c r="B10" s="63"/>
-      <c r="C10" s="63"/>
-      <c r="D10" s="63"/>
-      <c r="E10" s="63"/>
-      <c r="F10" s="63"/>
-      <c r="G10" s="64"/>
+      <c r="B10" s="60"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="60"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="61"/>
       <c r="H10" s="3"/>
       <c r="I10" s="8" t="s">
         <v>31</v>
@@ -2272,15 +2272,15 @@
       <c r="Z10" s="1"/>
     </row>
     <row r="11" spans="1:26" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A11" s="61">
+      <c r="A11" s="58">
         <v>9</v>
       </c>
-      <c r="B11" s="63"/>
-      <c r="C11" s="63"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="63"/>
-      <c r="G11" s="64"/>
+      <c r="B11" s="60"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="61"/>
       <c r="H11" s="3"/>
       <c r="I11" s="7" t="s">
         <v>32</v>
@@ -2306,15 +2306,15 @@
       <c r="Z11" s="1"/>
     </row>
     <row r="12" spans="1:26" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A12" s="61">
+      <c r="A12" s="58">
         <v>10</v>
       </c>
-      <c r="B12" s="63"/>
-      <c r="C12" s="63"/>
-      <c r="D12" s="63"/>
-      <c r="E12" s="63"/>
-      <c r="F12" s="63"/>
-      <c r="G12" s="64"/>
+      <c r="B12" s="60"/>
+      <c r="C12" s="60"/>
+      <c r="D12" s="60"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="61"/>
       <c r="H12" s="3"/>
       <c r="I12" s="7" t="s">
         <v>34</v>
@@ -2340,15 +2340,15 @@
       <c r="Z12" s="1"/>
     </row>
     <row r="13" spans="1:26" ht="14.1" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A13" s="61">
+      <c r="A13" s="58">
         <v>11</v>
       </c>
-      <c r="B13" s="63"/>
-      <c r="C13" s="63"/>
-      <c r="D13" s="63"/>
-      <c r="E13" s="63"/>
-      <c r="F13" s="63"/>
-      <c r="G13" s="64"/>
+      <c r="B13" s="60"/>
+      <c r="C13" s="60"/>
+      <c r="D13" s="60"/>
+      <c r="E13" s="60"/>
+      <c r="F13" s="60"/>
+      <c r="G13" s="61"/>
       <c r="H13" s="3"/>
       <c r="I13" s="7" t="s">
         <v>36</v>
@@ -2374,15 +2374,15 @@
       <c r="Z13" s="1"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="61">
+      <c r="A14" s="58">
         <v>12</v>
       </c>
-      <c r="B14" s="63"/>
-      <c r="C14" s="63"/>
-      <c r="D14" s="63"/>
-      <c r="E14" s="63"/>
-      <c r="F14" s="63"/>
-      <c r="G14" s="64"/>
+      <c r="B14" s="60"/>
+      <c r="C14" s="60"/>
+      <c r="D14" s="60"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="61"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -2404,15 +2404,15 @@
       <c r="Z14" s="1"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="61">
+      <c r="A15" s="58">
         <v>13</v>
       </c>
-      <c r="B15" s="63"/>
-      <c r="C15" s="63"/>
-      <c r="D15" s="63"/>
-      <c r="E15" s="63"/>
-      <c r="F15" s="63"/>
-      <c r="G15" s="64"/>
+      <c r="B15" s="60"/>
+      <c r="C15" s="60"/>
+      <c r="D15" s="60"/>
+      <c r="E15" s="60"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="61"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
@@ -2434,15 +2434,15 @@
       <c r="Z15" s="1"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="61">
+      <c r="A16" s="58">
         <v>14</v>
       </c>
-      <c r="B16" s="63"/>
-      <c r="C16" s="63"/>
-      <c r="D16" s="63"/>
-      <c r="E16" s="63"/>
-      <c r="F16" s="63"/>
-      <c r="G16" s="64"/>
+      <c r="B16" s="60"/>
+      <c r="C16" s="60"/>
+      <c r="D16" s="60"/>
+      <c r="E16" s="60"/>
+      <c r="F16" s="60"/>
+      <c r="G16" s="61"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -2464,15 +2464,15 @@
       <c r="Z16" s="1"/>
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="61">
+      <c r="A17" s="58">
         <v>15</v>
       </c>
-      <c r="B17" s="63"/>
-      <c r="C17" s="63"/>
-      <c r="D17" s="63"/>
-      <c r="E17" s="63"/>
-      <c r="F17" s="63"/>
-      <c r="G17" s="64"/>
+      <c r="B17" s="60"/>
+      <c r="C17" s="60"/>
+      <c r="D17" s="60"/>
+      <c r="E17" s="60"/>
+      <c r="F17" s="60"/>
+      <c r="G17" s="61"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -2494,30 +2494,30 @@
       <c r="Z17" s="1"/>
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="61" t="s">
+      <c r="A18" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="63">
+      <c r="B18" s="60">
         <f>SUM(B3:B8)</f>
         <v>0</v>
       </c>
-      <c r="C18" s="63">
+      <c r="C18" s="60">
         <f>SUM(C3:C8)</f>
         <v>0</v>
       </c>
-      <c r="D18" s="63">
+      <c r="D18" s="60">
         <f>SUM(D3:D8)</f>
         <v>0</v>
       </c>
-      <c r="E18" s="63">
+      <c r="E18" s="60">
         <f>SUM(E3:E8)</f>
         <v>0</v>
       </c>
-      <c r="F18" s="63">
+      <c r="F18" s="60">
         <f>SUM(F3:F8)</f>
         <v>0</v>
       </c>
-      <c r="G18" s="63"/>
+      <c r="G18" s="60"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>

</xml_diff>